<commit_message>
Clase 6 de junio Tarde
</commit_message>
<xml_diff>
--- a/Asistencia/Grupo 50.xlsx
+++ b/Asistencia/Grupo 50.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Monitorias\Asistencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CFA718-50A1-406B-B5A2-BA4D06A90430}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83257A4-8F01-454D-A1A3-10FC421FBCA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="80">
   <si>
     <t>SISTEMA DE REGISTRO ACADÉMICO Y ADMISIONES (SRA)</t>
   </si>
@@ -409,7 +409,7 @@
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="26">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -422,11 +422,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -472,6 +482,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -487,6 +507,156 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -878,12 +1048,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T37"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection activeCell="C3" sqref="C3"/>
-      <selection pane="topRight" activeCell="V7" sqref="V7"/>
+      <selection pane="topRight" activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -894,7 +1064,7 @@
     <col min="8" max="8" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -907,7 +1077,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -920,7 +1090,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -936,7 +1106,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -988,11 +1158,14 @@
       <c r="S4" s="9">
         <v>45076</v>
       </c>
-      <c r="T4" s="10" t="s">
+      <c r="T4" s="9">
+        <v>45083</v>
+      </c>
+      <c r="U4" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -1042,12 +1215,15 @@
       <c r="S5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T5">
-        <f>COUNTIF(I5:S5,"F")</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U5">
+        <f>COUNTIF(I5:T5,"F")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -1077,12 +1253,13 @@
       <c r="Q6" s="14"/>
       <c r="R6" s="11"/>
       <c r="S6" s="11"/>
-      <c r="T6">
-        <f>COUNTIF(I6:S6,"F")</f>
+      <c r="T6" s="11"/>
+      <c r="U6">
+        <f>COUNTIF(I6:T6,"F")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -1112,12 +1289,13 @@
       <c r="Q7" s="14"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
-      <c r="T7">
-        <f t="shared" ref="T7:T37" si="0">COUNTIF(I7:S7,"F")</f>
+      <c r="T7" s="11"/>
+      <c r="U7">
+        <f t="shared" ref="U7:U37" si="0">COUNTIF(I7:T7,"F")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -1147,12 +1325,13 @@
       <c r="Q8" s="14"/>
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
-      <c r="T8">
+      <c r="T8" s="11"/>
+      <c r="U8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -1184,12 +1363,13 @@
       <c r="S9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="11"/>
+      <c r="U9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -1233,12 +1413,15 @@
       <c r="S10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T10">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -1270,12 +1453,13 @@
       <c r="Q11" s="14"/>
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
-      <c r="T11">
+      <c r="T11" s="11"/>
+      <c r="U11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -1305,12 +1489,13 @@
       <c r="Q12" s="14"/>
       <c r="R12" s="11"/>
       <c r="S12" s="11"/>
-      <c r="T12">
+      <c r="T12" s="11"/>
+      <c r="U12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -1354,12 +1539,15 @@
       <c r="S13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T13">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -1389,12 +1577,13 @@
       <c r="Q14" s="14"/>
       <c r="R14" s="11"/>
       <c r="S14" s="11"/>
-      <c r="T14">
+      <c r="T14" s="11"/>
+      <c r="U14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>11</v>
       </c>
@@ -1442,12 +1631,15 @@
       <c r="S15" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T15">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>12</v>
       </c>
@@ -1479,12 +1671,15 @@
       <c r="Q16" s="14"/>
       <c r="R16" s="11"/>
       <c r="S16" s="11"/>
-      <c r="T16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>13</v>
       </c>
@@ -1518,12 +1713,13 @@
       <c r="S17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T17">
+      <c r="T17" s="11"/>
+      <c r="U17">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>14</v>
       </c>
@@ -1571,12 +1767,15 @@
       <c r="S18" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T18">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T18" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>15</v>
       </c>
@@ -1624,12 +1823,15 @@
       <c r="S19" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T19">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>16</v>
       </c>
@@ -1677,12 +1879,15 @@
       <c r="S20" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T20">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T20" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>17</v>
       </c>
@@ -1724,12 +1929,15 @@
       <c r="S21" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T21">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T21" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>18</v>
       </c>
@@ -1775,12 +1983,15 @@
       <c r="S22" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T22">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>19</v>
       </c>
@@ -1820,12 +2031,13 @@
         <v>12</v>
       </c>
       <c r="S23" s="11"/>
-      <c r="T23">
+      <c r="T23" s="11"/>
+      <c r="U23">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>20</v>
       </c>
@@ -1857,12 +2069,15 @@
       <c r="S24" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T24">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T24" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>21</v>
       </c>
@@ -1892,12 +2107,13 @@
       <c r="Q25" s="14"/>
       <c r="R25" s="11"/>
       <c r="S25" s="11"/>
-      <c r="T25">
+      <c r="T25" s="11"/>
+      <c r="U25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -1927,12 +2143,13 @@
       <c r="Q26" s="14"/>
       <c r="R26" s="11"/>
       <c r="S26" s="11"/>
-      <c r="T26">
+      <c r="T26" s="11"/>
+      <c r="U26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -1962,12 +2179,13 @@
       <c r="Q27" s="14"/>
       <c r="R27" s="11"/>
       <c r="S27" s="11"/>
-      <c r="T27">
+      <c r="T27" s="11"/>
+      <c r="U27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>25</v>
       </c>
@@ -1997,12 +2215,13 @@
       <c r="Q28" s="14"/>
       <c r="R28" s="11"/>
       <c r="S28" s="11"/>
-      <c r="T28">
+      <c r="T28" s="11"/>
+      <c r="U28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -2034,12 +2253,15 @@
       <c r="Q29" s="14"/>
       <c r="R29" s="11"/>
       <c r="S29" s="11"/>
-      <c r="T29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T29" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>27</v>
       </c>
@@ -2069,12 +2291,13 @@
       <c r="Q30" s="14"/>
       <c r="R30" s="11"/>
       <c r="S30" s="11"/>
-      <c r="T30">
+      <c r="T30" s="11"/>
+      <c r="U30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -2116,12 +2339,15 @@
       <c r="S31" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T31">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T31" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>29</v>
       </c>
@@ -2153,12 +2379,13 @@
       <c r="Q32" s="14"/>
       <c r="R32" s="11"/>
       <c r="S32" s="11"/>
-      <c r="T32">
+      <c r="T32" s="11"/>
+      <c r="U32">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -2198,12 +2425,15 @@
       <c r="S33" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T33">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>31</v>
       </c>
@@ -2233,12 +2463,13 @@
       <c r="Q34" s="14"/>
       <c r="R34" s="11"/>
       <c r="S34" s="11"/>
-      <c r="T34">
+      <c r="T34" s="11"/>
+      <c r="U34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>32</v>
       </c>
@@ -2286,12 +2517,15 @@
       <c r="S35" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T35">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T35" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>33</v>
       </c>
@@ -2339,12 +2573,15 @@
       <c r="S36" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T36">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>34</v>
       </c>
@@ -2392,9 +2629,12 @@
       <c r="S37" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T37">
-        <f t="shared" si="0"/>
-        <v>9</v>
+      <c r="T37" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2402,27 +2642,38 @@
     <mergeCell ref="L5:L37"/>
     <mergeCell ref="Q5:Q37"/>
   </mergeCells>
-  <conditionalFormatting sqref="I5:R37">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+  <conditionalFormatting sqref="I5:S37">
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:S37">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T5:T37">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="U5:U37">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="greaterThan">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S5:S37">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T5:T37">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>" "</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -2432,8 +2683,5 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
-  <ignoredErrors>
-    <ignoredError sqref="T5 T10:T11 T15:T23 T29 T31:T33 T35:T37" unlockedFormula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
28 de Junio 2023
</commit_message>
<xml_diff>
--- a/Asistencia/Grupo 50.xlsx
+++ b/Asistencia/Grupo 50.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Monitorias\Asistencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682E35BB-B6D4-4D90-8760-B8EB866A9B17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C415CF-54A4-4BE3-A8BC-794B7723CF58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="80">
   <si>
     <t>SISTEMA DE REGISTRO ACADÉMICO Y ADMISIONES (SRA)</t>
   </si>
@@ -409,7 +409,147 @@
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1008,12 +1148,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X37"/>
+  <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
       <selection activeCell="C3" sqref="C3"/>
-      <selection pane="topRight" activeCell="Q5" sqref="Q5:Q37"/>
+      <selection pane="topRight" activeCell="X34" sqref="X34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1024,7 +1164,7 @@
     <col min="8" max="8" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1037,7 +1177,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1050,7 +1190,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1066,7 +1206,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1130,11 +1270,14 @@
       <c r="W4" s="9">
         <v>45097</v>
       </c>
-      <c r="X4" s="10" t="s">
+      <c r="X4" s="9">
+        <v>45103</v>
+      </c>
+      <c r="Y4" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -1196,12 +1339,15 @@
       <c r="W5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X5">
+      <c r="X5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y5">
         <f>COUNTIF(I5:W5,"F")</f>
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -1235,12 +1381,13 @@
       <c r="U6" s="11"/>
       <c r="V6" s="11"/>
       <c r="W6" s="11"/>
-      <c r="X6">
+      <c r="X6" s="11"/>
+      <c r="Y6">
         <f>COUNTIF(I6:W6,"F")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -1274,12 +1421,13 @@
       <c r="U7" s="11"/>
       <c r="V7" s="11"/>
       <c r="W7" s="11"/>
-      <c r="X7">
-        <f t="shared" ref="X7:X37" si="0">COUNTIF(I7:W7,"F")</f>
+      <c r="X7" s="11"/>
+      <c r="Y7">
+        <f>COUNTIF(I7:W7,"F")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -1313,12 +1461,13 @@
       <c r="U8" s="11"/>
       <c r="V8" s="11"/>
       <c r="W8" s="11"/>
-      <c r="X8">
-        <f t="shared" si="0"/>
+      <c r="X8" s="11"/>
+      <c r="Y8">
+        <f>COUNTIF(I8:W8,"F")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -1354,12 +1503,13 @@
       <c r="U9" s="11"/>
       <c r="V9" s="11"/>
       <c r="W9" s="11"/>
-      <c r="X9">
-        <f t="shared" si="0"/>
+      <c r="X9" s="11"/>
+      <c r="Y9">
+        <f>COUNTIF(I9:W9,"F")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -1415,12 +1565,15 @@
       <c r="W10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X10">
-        <f t="shared" si="0"/>
+      <c r="X10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y10">
+        <f>COUNTIF(I10:W10,"F")</f>
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -1458,12 +1611,15 @@
       <c r="W11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X11">
-        <f t="shared" si="0"/>
+      <c r="X11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y11">
+        <f>COUNTIF(I11:W11,"F")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -1497,12 +1653,13 @@
       <c r="U12" s="11"/>
       <c r="V12" s="11"/>
       <c r="W12" s="11"/>
-      <c r="X12">
-        <f t="shared" si="0"/>
+      <c r="X12" s="11"/>
+      <c r="Y12">
+        <f>COUNTIF(I12:W12,"F")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -1558,12 +1715,15 @@
       <c r="W13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X13">
-        <f t="shared" si="0"/>
+      <c r="X13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y13">
+        <f>COUNTIF(I13:W13,"F")</f>
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -1597,12 +1757,13 @@
       <c r="U14" s="11"/>
       <c r="V14" s="11"/>
       <c r="W14" s="11"/>
-      <c r="X14">
-        <f t="shared" si="0"/>
+      <c r="X14" s="11"/>
+      <c r="Y14">
+        <f>COUNTIF(I14:W14,"F")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>11</v>
       </c>
@@ -1662,12 +1823,15 @@
       <c r="W15" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X15">
-        <f t="shared" si="0"/>
+      <c r="X15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y15">
+        <f>COUNTIF(I15:W15,"F")</f>
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>12</v>
       </c>
@@ -1711,12 +1875,15 @@
       <c r="W16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X16">
-        <f t="shared" si="0"/>
+      <c r="X16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y16">
+        <f>COUNTIF(I16:W16,"F")</f>
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>13</v>
       </c>
@@ -1754,12 +1921,13 @@
       <c r="U17" s="11"/>
       <c r="V17" s="11"/>
       <c r="W17" s="11"/>
-      <c r="X17">
-        <f t="shared" si="0"/>
+      <c r="X17" s="11"/>
+      <c r="Y17">
+        <f>COUNTIF(I17:W17,"F")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>14</v>
       </c>
@@ -1819,12 +1987,15 @@
       <c r="W18" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X18">
-        <f t="shared" si="0"/>
+      <c r="X18" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y18">
+        <f>COUNTIF(I18:W18,"F")</f>
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>15</v>
       </c>
@@ -1884,12 +2055,15 @@
       <c r="W19" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X19">
-        <f t="shared" si="0"/>
+      <c r="X19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y19">
+        <f>COUNTIF(I19:W19,"F")</f>
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>16</v>
       </c>
@@ -1949,12 +2123,15 @@
       <c r="W20" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X20">
-        <f t="shared" si="0"/>
+      <c r="X20" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y20">
+        <f>COUNTIF(I20:W20,"F")</f>
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>17</v>
       </c>
@@ -2008,12 +2185,15 @@
       <c r="W21" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X21">
-        <f t="shared" si="0"/>
+      <c r="X21" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y21">
+        <f>COUNTIF(I21:W21,"F")</f>
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>18</v>
       </c>
@@ -2071,12 +2251,15 @@
       <c r="W22" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X22">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y22">
+        <f>COUNTIF(I22:W22,"F")</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>19</v>
       </c>
@@ -2120,12 +2303,13 @@
       <c r="U23" s="11"/>
       <c r="V23" s="11"/>
       <c r="W23" s="11"/>
-      <c r="X23">
-        <f t="shared" si="0"/>
+      <c r="X23" s="11"/>
+      <c r="Y23">
+        <f>COUNTIF(I23:W23,"F")</f>
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>20</v>
       </c>
@@ -2167,12 +2351,15 @@
       <c r="W24" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X24">
-        <f t="shared" si="0"/>
+      <c r="X24" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y24">
+        <f>COUNTIF(I24:W24,"F")</f>
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>21</v>
       </c>
@@ -2206,12 +2393,13 @@
       <c r="U25" s="11"/>
       <c r="V25" s="11"/>
       <c r="W25" s="11"/>
-      <c r="X25">
-        <f t="shared" si="0"/>
+      <c r="X25" s="11"/>
+      <c r="Y25">
+        <f>COUNTIF(I25:W25,"F")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -2245,12 +2433,13 @@
       <c r="U26" s="11"/>
       <c r="V26" s="11"/>
       <c r="W26" s="11"/>
-      <c r="X26">
-        <f t="shared" si="0"/>
+      <c r="X26" s="11"/>
+      <c r="Y26">
+        <f>COUNTIF(I26:W26,"F")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -2284,12 +2473,13 @@
       <c r="U27" s="11"/>
       <c r="V27" s="11"/>
       <c r="W27" s="11"/>
-      <c r="X27">
-        <f t="shared" si="0"/>
+      <c r="X27" s="11"/>
+      <c r="Y27">
+        <f>COUNTIF(I27:W27,"F")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>25</v>
       </c>
@@ -2323,12 +2513,13 @@
       <c r="U28" s="11"/>
       <c r="V28" s="11"/>
       <c r="W28" s="11"/>
-      <c r="X28">
-        <f t="shared" si="0"/>
+      <c r="X28" s="11"/>
+      <c r="Y28">
+        <f>COUNTIF(I28:W28,"F")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -2365,15 +2556,14 @@
         <v>12</v>
       </c>
       <c r="V29" s="11"/>
-      <c r="W29" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="X29">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W29" s="11"/>
+      <c r="X29" s="11"/>
+      <c r="Y29">
+        <f>COUNTIF(I29:W29,"F")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>27</v>
       </c>
@@ -2407,12 +2597,13 @@
       <c r="U30" s="11"/>
       <c r="V30" s="11"/>
       <c r="W30" s="11"/>
-      <c r="X30">
-        <f t="shared" si="0"/>
+      <c r="X30" s="11"/>
+      <c r="Y30">
+        <f>COUNTIF(I30:W30,"F")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -2466,12 +2657,15 @@
       <c r="W31" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X31">
-        <f t="shared" si="0"/>
+      <c r="X31" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y31">
+        <f>COUNTIF(I31:W31,"F")</f>
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>29</v>
       </c>
@@ -2509,12 +2703,15 @@
       <c r="W32" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X32">
-        <f t="shared" si="0"/>
+      <c r="X32" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y32">
+        <f>COUNTIF(I32:W32,"F")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -2566,12 +2763,15 @@
       <c r="W33" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X33">
-        <f t="shared" si="0"/>
+      <c r="X33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y33">
+        <f>COUNTIF(I33:W33,"F")</f>
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>31</v>
       </c>
@@ -2607,12 +2807,13 @@
       <c r="W34" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X34">
-        <f t="shared" si="0"/>
+      <c r="X34" s="11"/>
+      <c r="Y34">
+        <f>COUNTIF(I34:W34,"F")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>32</v>
       </c>
@@ -2672,12 +2873,15 @@
       <c r="W35" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X35">
-        <f t="shared" si="0"/>
+      <c r="X35" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y35">
+        <f>COUNTIF(I35:W35,"F")</f>
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>33</v>
       </c>
@@ -2737,12 +2941,15 @@
       <c r="W36" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X36">
-        <f t="shared" si="0"/>
+      <c r="X36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y36">
+        <f>COUNTIF(I36:W36,"F")</f>
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>34</v>
       </c>
@@ -2802,8 +3009,11 @@
       <c r="W37" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="X37">
-        <f t="shared" si="0"/>
+      <c r="X37" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y37">
+        <f>COUNTIF(I37:W37,"F")</f>
         <v>13</v>
       </c>
     </row>
@@ -2813,45 +3023,103 @@
     <mergeCell ref="Q5:Q37"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:U37">
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:U37">
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="34" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="lessThan">
       <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y5:Y37">
+    <cfRule type="cellIs" dxfId="32" priority="33" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S5:U37">
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U5:U37">
+    <cfRule type="cellIs" dxfId="30" priority="29" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
+      <formula>" "</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W5:W37">
+    <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W5:W37">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W5:W37">
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W5:W37">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+      <formula>" "</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V5:W37">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V5:W37">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V5:W37">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V5:W37">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+      <formula>" "</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
+      <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X5:X37">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="greaterThan">
-      <formula>4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S5:U37">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U5:U37">
-    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
-      <formula>" "</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W5:W37">
     <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W5:W37">
+  <conditionalFormatting sqref="X5:X37">
     <cfRule type="cellIs" dxfId="12" priority="12" operator="lessThan">
       <formula>1</formula>
     </cfRule>
@@ -2859,12 +3127,12 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W5:W37">
+  <conditionalFormatting sqref="X5:X37">
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W5:W37">
+  <conditionalFormatting sqref="X5:X37">
     <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -2875,12 +3143,12 @@
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V5:V37">
+  <conditionalFormatting sqref="X5:X37">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V5:V37">
+  <conditionalFormatting sqref="X5:X37">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
       <formula>1</formula>
     </cfRule>
@@ -2888,12 +3156,12 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V5:V37">
+  <conditionalFormatting sqref="X5:X37">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V5:V37">
+  <conditionalFormatting sqref="X5:X37">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>